<commit_message>
modified Advanced search data dependancy classes
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="createManufacturer" sheetId="1" r:id="rId1"/>
-    <sheet name="verifyWelcome" sheetId="2" r:id="rId2"/>
+    <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
+    <sheet name="createNewBrand" sheetId="2" r:id="rId2"/>
+    <sheet name="createNewSubset" sheetId="3" r:id="rId3"/>
+    <sheet name="createNewItem" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>User name</t>
   </si>
@@ -57,6 +59,78 @@
   </si>
   <si>
     <t>Welcome, cimm-vadiraja !</t>
+  </si>
+  <si>
+    <t>BrandName</t>
+  </si>
+  <si>
+    <t>Brand Description</t>
+  </si>
+  <si>
+    <t>Sucessful Message After Brand creation</t>
+  </si>
+  <si>
+    <t>AS_Brand_Automation_Testing</t>
+  </si>
+  <si>
+    <t>Test for automation</t>
+  </si>
+  <si>
+    <t>Brand saved Successfully</t>
+  </si>
+  <si>
+    <t>tc_advancedSearch_002</t>
+  </si>
+  <si>
+    <t>Subset Name</t>
+  </si>
+  <si>
+    <t>Successful message for newly created Subset</t>
+  </si>
+  <si>
+    <t>New Subset saved Successfully</t>
+  </si>
+  <si>
+    <t>AS_Automation_Subset</t>
+  </si>
+  <si>
+    <t>tc_advancedSearch_003</t>
+  </si>
+  <si>
+    <t>Mfg Name</t>
+  </si>
+  <si>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Item name template</t>
+  </si>
+  <si>
+    <t>mfg name template</t>
+  </si>
+  <si>
+    <t>vendor name</t>
+  </si>
+  <si>
+    <t>successful message for created Item</t>
+  </si>
+  <si>
+    <t>no of items to be create</t>
+  </si>
+  <si>
+    <t>AS_Automation_Supplier</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Automation_PN</t>
+  </si>
+  <si>
+    <t>Automation_MPN</t>
+  </si>
+  <si>
+    <t>Item saved Successfully</t>
   </si>
 </sst>
 </file>
@@ -86,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,15 +183,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +514,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E2" activeCellId="1" sqref="E1 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,10 +581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,9 +593,13 @@
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -519,10 +612,22 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -532,6 +637,183 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Advance search Data till TC_11
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,20 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
     <sheet name="createNewBrand" sheetId="2" r:id="rId2"/>
     <sheet name="createNewSubset" sheetId="3" r:id="rId3"/>
     <sheet name="createNewItem" sheetId="4" r:id="rId4"/>
+    <sheet name="advSearch_004" sheetId="6" r:id="rId5"/>
+    <sheet name="advSearch_005" sheetId="7" r:id="rId6"/>
+    <sheet name="advSearch_003" sheetId="5" r:id="rId7"/>
+    <sheet name="advSearch_006" sheetId="8" r:id="rId8"/>
+    <sheet name="advSearch_007" sheetId="9" r:id="rId9"/>
+    <sheet name="advSearch_008" sheetId="10" r:id="rId10"/>
+    <sheet name="advSearch_009" sheetId="11" r:id="rId11"/>
+    <sheet name="advSearch_010" sheetId="12" r:id="rId12"/>
+    <sheet name="advSearch_011" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="65">
   <si>
     <t>User name</t>
   </si>
@@ -37,12 +46,6 @@
     <t>Successful message After creation Mfg</t>
   </si>
   <si>
-    <t>unilogvadi</t>
-  </si>
-  <si>
-    <t>vadiraja</t>
-  </si>
-  <si>
     <t>AS_Manufacturer_Automation_Testing</t>
   </si>
   <si>
@@ -58,9 +61,6 @@
     <t>tc_advancedSearch_001</t>
   </si>
   <si>
-    <t>Welcome, cimm-vadiraja !</t>
-  </si>
-  <si>
     <t>BrandName</t>
   </si>
   <si>
@@ -131,6 +131,96 @@
   </si>
   <si>
     <t>Item saved Successfully</t>
+  </si>
+  <si>
+    <t>TestCase_ID</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Search Data</t>
+  </si>
+  <si>
+    <t>automationUser</t>
+  </si>
+  <si>
+    <t>unilog123##</t>
+  </si>
+  <si>
+    <t>Automation_PN_1</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_003</t>
+  </si>
+  <si>
+    <t>Welcome, Automation !</t>
+  </si>
+  <si>
+    <t>Invalid Partial Part No or keyword</t>
+  </si>
+  <si>
+    <t>Search Dat</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_004</t>
+  </si>
+  <si>
+    <t>Expected Message</t>
+  </si>
+  <si>
+    <t>No Items Found</t>
+  </si>
+  <si>
+    <t>Invalid keyword</t>
+  </si>
+  <si>
+    <t>Automation_PN_2</t>
+  </si>
+  <si>
+    <t>SearchData</t>
+  </si>
+  <si>
+    <t>Select Value</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_007</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_008</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_009</t>
+  </si>
+  <si>
+    <t>Invalid Part number</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_010</t>
+  </si>
+  <si>
+    <t>Automation_MPN_4</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_011</t>
+  </si>
+  <si>
+    <t>Invalid Manufacturer Part No</t>
   </si>
 </sst>
 </file>
@@ -146,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -207,6 +303,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +615,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="E1 E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +623,7 @@
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="24.140625" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" customWidth="1"/>
@@ -530,7 +631,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -553,25 +654,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -579,9 +680,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -589,10 +690,248 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.5703125" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.140625" customWidth="1"/>
@@ -601,7 +940,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -616,39 +955,39 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -661,22 +1000,22 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -688,30 +1027,30 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -723,16 +1062,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -742,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -754,66 +1093,326 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>34</v>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified test scripte in ADNS
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,18 @@
     <sheet name="advSearch_009" sheetId="11" r:id="rId11"/>
     <sheet name="advSearch_010" sheetId="12" r:id="rId12"/>
     <sheet name="advSearch_011" sheetId="13" r:id="rId13"/>
+    <sheet name="advSearch_014" sheetId="14" r:id="rId14"/>
+    <sheet name="advSe015" sheetId="15" r:id="rId15"/>
+    <sheet name="advSe016" sheetId="16" r:id="rId16"/>
+    <sheet name="advSearch_017" sheetId="17" r:id="rId17"/>
+    <sheet name="advSearch_018" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
   <si>
     <t>User name</t>
   </si>
@@ -221,6 +226,30 @@
   </si>
   <si>
     <t>Invalid Manufacturer Part No</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_014</t>
+  </si>
+  <si>
+    <t>Automation_PN_3</t>
+  </si>
+  <si>
+    <t>CIMM Item Id</t>
+  </si>
+  <si>
+    <t>Invalid CIMM item ID</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_015</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_016</t>
+  </si>
+  <si>
+    <t>No of items to create</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_017</t>
   </si>
 </sst>
 </file>
@@ -615,7 +644,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,6 +940,314 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1502,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed data provider classes in advanced search module
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QA/UnilogProjects/cimm2touch/resources/ExcelsheetData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="19" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -25,13 +30,33 @@
     <sheet name="advSe016" sheetId="16" r:id="rId16"/>
     <sheet name="advSearch_017" sheetId="17" r:id="rId17"/>
     <sheet name="advSearch_018" sheetId="18" r:id="rId18"/>
+    <sheet name="advSe019" sheetId="19" r:id="rId19"/>
+    <sheet name="advSearch_020" sheetId="20" r:id="rId20"/>
+    <sheet name="advSearch_021" sheetId="21" r:id="rId21"/>
+    <sheet name="advSearch_022" sheetId="22" r:id="rId22"/>
+    <sheet name="advSearch_023" sheetId="23" r:id="rId23"/>
+    <sheet name="advSearch_024" sheetId="24" r:id="rId24"/>
+    <sheet name="advSearch_025" sheetId="25" r:id="rId25"/>
+    <sheet name="advSearch_026" sheetId="26" r:id="rId26"/>
+    <sheet name="advSearch_027" sheetId="27" r:id="rId27"/>
+    <sheet name="advSearch_028" sheetId="28" r:id="rId28"/>
+    <sheet name="addDescriptiontoItems" sheetId="29" r:id="rId29"/>
+    <sheet name="addImageURLtoItems" sheetId="30" r:id="rId30"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="106">
   <si>
     <t>User name</t>
   </si>
@@ -250,6 +275,105 @@
   </si>
   <si>
     <t>TC_ADV SEARCH_017</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_019</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_018</t>
+  </si>
+  <si>
+    <t>Item Name Template</t>
+  </si>
+  <si>
+    <t>NoOf Items To Be created</t>
+  </si>
+  <si>
+    <t>Manufacture Temlate</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_020</t>
+  </si>
+  <si>
+    <t>Automation_PN_</t>
+  </si>
+  <si>
+    <t>Automation_MPN_</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_021</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_022</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_023</t>
+  </si>
+  <si>
+    <t>Select Item Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_024</t>
+  </si>
+  <si>
+    <t>Display online Status</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_025</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_026</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_027</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_028</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_029</t>
+  </si>
+  <si>
+    <t>Welcome Message</t>
+  </si>
+  <si>
+    <t>Part Number Description</t>
+  </si>
+  <si>
+    <t>Long Desc1</t>
+  </si>
+  <si>
+    <t>Long Desc2</t>
+  </si>
+  <si>
+    <t>This is the long Description 1.</t>
+  </si>
+  <si>
+    <t>This is the long Description 2.</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_030</t>
+  </si>
+  <si>
+    <t>Image URL</t>
+  </si>
+  <si>
+    <t>https://www.nasa.gov/sites/default/files/styles/image_card_4x3_ratio/public/thumbnails/image/nh-global-water-ice.jpg</t>
   </si>
 </sst>
 </file>
@@ -295,25 +419,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -400,9 +524,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -435,9 +559,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -647,18 +771,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -681,7 +805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -717,16 +841,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -743,7 +867,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -773,17 +897,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -803,7 +927,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -836,16 +960,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -862,7 +986,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -892,17 +1016,17 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -922,7 +1046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -955,16 +1079,16 @@
       <selection activeCell="A3" sqref="A3:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -981,7 +1105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -1011,17 +1135,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1165,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
@@ -1074,17 +1198,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1104,7 +1228,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1137,17 +1261,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1167,7 +1291,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1196,21 +1320,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1230,9 +1354,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -1255,6 +1379,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
@@ -1263,19 +1450,19 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1301,7 +1488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1332,6 +1519,612 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
@@ -1340,17 +2133,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +2163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1395,6 +2188,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
@@ -1403,20 +2259,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="24.5703125" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1454,7 +2310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1505,16 +2361,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +2387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1561,12 +2417,12 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1580,7 +2436,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1607,15 +2463,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +2485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -1656,13 +2512,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1679,7 +2535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1709,16 +2565,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1735,7 +2591,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
modified test scripts till Tc_32
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QA/UnilogProjects/cimm2touch/resources/ExcelsheetData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="19" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="25" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -42,12 +37,11 @@
     <sheet name="advSearch_028" sheetId="28" r:id="rId28"/>
     <sheet name="addDescriptiontoItems" sheetId="29" r:id="rId29"/>
     <sheet name="addImageURLtoItems" sheetId="30" r:id="rId30"/>
+    <sheet name="advSearch_29" sheetId="32" r:id="rId31"/>
+    <sheet name="addDocumenttoItems" sheetId="31" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -56,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="111">
   <si>
     <t>User name</t>
   </si>
@@ -374,6 +368,21 @@
   </si>
   <si>
     <t>https://www.nasa.gov/sites/default/files/styles/image_card_4x3_ratio/public/thumbnails/image/nh-global-water-ice.jpg</t>
+  </si>
+  <si>
+    <t>Document Location</t>
+  </si>
+  <si>
+    <t>resourceLocation+"Document.docx"</t>
+  </si>
+  <si>
+    <t>Subset Status</t>
+  </si>
+  <si>
+    <t>InActive</t>
+  </si>
+  <si>
+    <t>Expected Items</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -461,6 +470,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,18 +785,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" customWidth="1"/>
-    <col min="7" max="7" width="39.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,7 +819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -841,16 +855,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -867,7 +881,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -897,17 +911,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -927,7 +941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -960,16 +974,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -986,7 +1000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1016,17 +1030,17 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1046,7 +1060,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -1079,16 +1093,16 @@
       <selection activeCell="A3" sqref="A3:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1119,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -1135,17 +1149,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1165,7 +1179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
@@ -1198,17 +1212,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1228,7 +1242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1261,17 +1275,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1291,7 +1305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1324,17 +1338,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1368,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -1387,17 +1401,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
@@ -1450,19 +1464,19 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1488,7 +1502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1527,16 +1541,16 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1573,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
@@ -1595,18 +1609,18 @@
       <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1629,7 +1643,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -1665,18 +1679,18 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1713,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -1735,17 +1749,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1768,7 +1782,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1804,15 +1818,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1826,7 +1840,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1853,15 +1867,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1875,7 +1889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1902,15 +1916,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1924,7 +1938,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>92</v>
       </c>
@@ -1951,15 +1965,15 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1987,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>93</v>
       </c>
@@ -2000,14 +2014,14 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2018,7 +2032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -2042,16 +2056,16 @@
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2074,7 +2088,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>96</v>
       </c>
@@ -2097,7 +2111,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>96</v>
       </c>
@@ -2133,17 +2147,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2177,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2192,21 +2206,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2222,11 +2236,11 @@
       <c r="E1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>103</v>
       </c>
@@ -2242,7 +2256,7 @@
       <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2251,6 +2265,206 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
@@ -2259,20 +2473,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2310,7 +2524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2361,16 +2575,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2387,7 +2601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2417,12 +2631,12 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2436,7 +2650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2463,15 +2677,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
@@ -2485,7 +2699,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -2512,13 +2726,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2535,7 +2749,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2565,16 +2779,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2591,7 +2805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Added test data till TC_40
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QA/UnilogProjects/cimm2touch/resources/ExcelsheetData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="25" activeTab="31"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" firstSheet="25" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -39,9 +44,15 @@
     <sheet name="addImageURLtoItems" sheetId="30" r:id="rId30"/>
     <sheet name="advSearch_29" sheetId="32" r:id="rId31"/>
     <sheet name="addDocumenttoItems" sheetId="31" r:id="rId32"/>
+    <sheet name="advSe033" sheetId="33" r:id="rId33"/>
+    <sheet name="advSe039" sheetId="34" r:id="rId34"/>
+    <sheet name="advSearch_040" sheetId="35" r:id="rId35"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -50,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="115">
   <si>
     <t>User name</t>
   </si>
@@ -383,6 +394,18 @@
   </si>
   <si>
     <t>Expected Items</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_033</t>
+  </si>
+  <si>
+    <t>advSesearchinput</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_039</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_040</t>
   </si>
 </sst>
 </file>
@@ -785,18 +808,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -819,7 +842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -855,16 +878,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -881,7 +904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -911,17 +934,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -941,7 +964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -974,16 +997,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1023,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1030,17 +1053,17 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -1093,16 +1116,16 @@
       <selection activeCell="A3" sqref="A3:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1142,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -1149,17 +1172,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1202,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
@@ -1212,17 +1235,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1265,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1275,17 +1298,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1338,17 +1361,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -1401,17 +1424,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1431,7 +1454,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
@@ -1464,19 +1487,19 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1502,7 +1525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1541,16 +1564,16 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1573,7 +1596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
@@ -1609,18 +1632,18 @@
       <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1643,7 +1666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -1679,18 +1702,18 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1713,7 +1736,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -1749,17 +1772,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1782,7 +1805,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1818,15 +1841,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1840,7 +1863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1867,15 +1890,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1889,7 +1912,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1916,15 +1939,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1938,7 +1961,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>92</v>
       </c>
@@ -1965,15 +1988,15 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1987,7 +2010,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>93</v>
       </c>
@@ -2014,14 +2037,14 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2032,7 +2055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -2056,16 +2079,16 @@
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2111,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>96</v>
       </c>
@@ -2111,7 +2134,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>96</v>
       </c>
@@ -2147,17 +2170,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2177,7 +2200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2206,21 +2229,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="112.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +2263,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>103</v>
       </c>
@@ -2273,18 +2296,18 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -2307,7 +2330,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>103</v>
       </c>
@@ -2330,7 +2353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -2353,7 +2376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>103</v>
       </c>
@@ -2386,21 +2409,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2420,7 +2443,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>103</v>
       </c>
@@ -2440,7 +2463,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
@@ -2465,6 +2488,228 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
@@ -2473,20 +2718,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2575,16 +2820,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2601,7 +2846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2631,12 +2876,12 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2650,7 +2895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2677,15 +2922,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
@@ -2699,7 +2944,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -2726,13 +2971,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2749,7 +2994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2779,16 +3024,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +3050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
modified testcases 31 to 45
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="30" activeTab="32"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="32" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,9 @@
     <sheet name="advSearch_29" sheetId="32" r:id="rId31"/>
     <sheet name="addDocumenttoItems" sheetId="31" r:id="rId32"/>
     <sheet name="advSearch_033_034_035" sheetId="33" r:id="rId33"/>
-    <sheet name="advSe039" sheetId="34" r:id="rId34"/>
+    <sheet name="advSearch_039" sheetId="34" r:id="rId34"/>
     <sheet name="advSearch_30_31_32" sheetId="39" r:id="rId35"/>
-    <sheet name="advSearch_040" sheetId="35" r:id="rId36"/>
+    <sheet name="advSearch_039_040_041" sheetId="35" r:id="rId36"/>
     <sheet name="advSearch_041" sheetId="36" r:id="rId37"/>
     <sheet name="advSearch_045_46" sheetId="37" r:id="rId38"/>
   </sheets>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="140">
   <si>
     <t>User name</t>
   </si>
@@ -446,6 +446,36 @@
   </si>
   <si>
     <t>Exp msg for No Attribute</t>
+  </si>
+  <si>
+    <t>Image Status</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>No Images</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_034</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_035</t>
+  </si>
+  <si>
+    <t>attributeValue</t>
+  </si>
+  <si>
+    <t>expErrormsgForNoAttribute</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>No LongDesc</t>
+  </si>
+  <si>
+    <t>LongDesc</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2105,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2481,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,9 +2574,10 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2562,8 +2593,11 @@
       <c r="E1" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
@@ -2579,6 +2613,49 @@
       <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2590,7 +2667,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +2750,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,10 +2846,126 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,69 +3000,6 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2975,10 +3105,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,9 +3118,12 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="109.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3007,10 +3140,19 @@
         <v>75</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -3024,13 +3166,22 @@
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>118</v>
       </c>
@@ -3044,10 +3195,19 @@
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>121</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test data for cimm2v4
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="32" activeTab="37"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="33" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,9 @@
     <sheet name="advSearch_30_31_32" sheetId="39" r:id="rId35"/>
     <sheet name="advSearch_039_040_041" sheetId="35" r:id="rId36"/>
     <sheet name="advSearch_041" sheetId="36" r:id="rId37"/>
-    <sheet name="advSearch_045_46" sheetId="37" r:id="rId38"/>
+    <sheet name="advSearch_042_043_044" sheetId="40" r:id="rId38"/>
+    <sheet name="deleteCreatedItem" sheetId="41" r:id="rId39"/>
+    <sheet name="advSearch_045_46" sheetId="37" r:id="rId40"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="151">
   <si>
     <t>User name</t>
   </si>
@@ -476,6 +478,39 @@
   </si>
   <si>
     <t>LongDesc</t>
+  </si>
+  <si>
+    <t>CategoryStatus</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_042</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_043</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_044</t>
+  </si>
+  <si>
+    <t>UnCategorized</t>
+  </si>
+  <si>
+    <t>Categorized</t>
+  </si>
+  <si>
+    <t>NoOfItems to be verify</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_deletePartNumber</t>
+  </si>
+  <si>
+    <t>Succesful message for deletion</t>
+  </si>
+  <si>
+    <t>Item with Part No. : '' removed Successfully</t>
+  </si>
+  <si>
+    <t>No Of Items to delete</t>
   </si>
 </sst>
 </file>
@@ -2965,7 +3000,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,10 +3140,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,13 +3152,11 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="109.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3137,24 +3170,15 @@
         <v>97</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3166,24 +3190,15 @@
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -3195,19 +3210,100 @@
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3316,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,6 +3413,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="109.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>

</xml_diff>

<commit_message>
added remove methods for created test data
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="33" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="37" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,10 @@
     <sheet name="advSearch_041" sheetId="36" r:id="rId37"/>
     <sheet name="advSearch_042_043_044" sheetId="40" r:id="rId38"/>
     <sheet name="deleteCreatedItem" sheetId="41" r:id="rId39"/>
-    <sheet name="advSearch_045_46" sheetId="37" r:id="rId40"/>
+    <sheet name="deleteCreatedBrand" sheetId="42" r:id="rId40"/>
+    <sheet name="deleteCreatedSubset" sheetId="43" r:id="rId41"/>
+    <sheet name="advSearch_045_46" sheetId="37" r:id="rId42"/>
+    <sheet name="deleteCreatedManufactures" sheetId="44" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="156">
   <si>
     <t>User name</t>
   </si>
@@ -511,6 +514,21 @@
   </si>
   <si>
     <t>No Of Items to delete</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_deleteBrand</t>
+  </si>
+  <si>
+    <t>tc_advancedSearch_deleteSubset</t>
+  </si>
+  <si>
+    <t>Manufacturer removed Successfully(No Brands and Items were present under this manufacturer).</t>
+  </si>
+  <si>
+    <t>SuccessMessage Deletion</t>
+  </si>
+  <si>
+    <t>TC_ADV SEARCH_deleteManufacturer</t>
   </si>
 </sst>
 </file>
@@ -584,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -604,6 +622,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1590,7 +1613,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2296,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3245,8 +3268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,7 +3339,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3390,10 +3413,10 @@
         <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>30</v>
@@ -3415,10 +3438,129 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,6 +3667,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>

</xml_diff>

<commit_message>
added remove methods for test data
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="37" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="24" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="advSearch_022" sheetId="22" r:id="rId22"/>
     <sheet name="advSearch_023" sheetId="23" r:id="rId23"/>
     <sheet name="advSearch_024" sheetId="24" r:id="rId24"/>
-    <sheet name="advSearch_025" sheetId="25" r:id="rId25"/>
+    <sheet name="advSearch_025_026_027" sheetId="25" r:id="rId25"/>
     <sheet name="advSearch_026" sheetId="26" r:id="rId26"/>
     <sheet name="advSearch_027" sheetId="27" r:id="rId27"/>
     <sheet name="advSearch_028" sheetId="28" r:id="rId28"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="158">
   <si>
     <t>User name</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>TC_ADV SEARCH_deleteManufacturer</t>
+  </si>
+  <si>
+    <t>No Of Items to be verify</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -627,6 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2013,21 +2020,22 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2040,8 +2048,11 @@
       <c r="D1" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -2053,6 +2064,43 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>89</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added vendor remove method
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QA/UnilogProjects/cimm2touch/resources/ExcelsheetData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="24" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23160" windowHeight="12840" firstSheet="25" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -38,23 +43,27 @@
     <sheet name="advSearch_028" sheetId="28" r:id="rId29"/>
     <sheet name="addDescriptiontoItems" sheetId="29" r:id="rId30"/>
     <sheet name="createVendor" sheetId="46" r:id="rId31"/>
-    <sheet name="addImageURLtoItems" sheetId="30" r:id="rId32"/>
-    <sheet name="advSearch_29" sheetId="32" r:id="rId33"/>
-    <sheet name="addDocumenttoItems" sheetId="31" r:id="rId34"/>
-    <sheet name="advSearch_033_034_035" sheetId="33" r:id="rId35"/>
-    <sheet name="advSearch_039" sheetId="34" r:id="rId36"/>
-    <sheet name="advSearch_30_31_32" sheetId="39" r:id="rId37"/>
-    <sheet name="advSearch_039_040_041" sheetId="35" r:id="rId38"/>
-    <sheet name="advSearch_041" sheetId="36" r:id="rId39"/>
-    <sheet name="advSearch_042_043_044" sheetId="40" r:id="rId40"/>
-    <sheet name="deleteCreatedItem" sheetId="41" r:id="rId41"/>
-    <sheet name="deleteCreatedBrand" sheetId="42" r:id="rId42"/>
-    <sheet name="deleteCreatedSubset" sheetId="43" r:id="rId43"/>
-    <sheet name="advSearch_045_46" sheetId="37" r:id="rId44"/>
-    <sheet name="deleteCreatedManufactures" sheetId="44" r:id="rId45"/>
+    <sheet name="deleteCreatedVendor" sheetId="47" r:id="rId32"/>
+    <sheet name="addImageURLtoItems" sheetId="30" r:id="rId33"/>
+    <sheet name="advSearch_29" sheetId="32" r:id="rId34"/>
+    <sheet name="addDocumenttoItems" sheetId="31" r:id="rId35"/>
+    <sheet name="advSearch_033_034_035" sheetId="33" r:id="rId36"/>
+    <sheet name="advSearch_039" sheetId="34" r:id="rId37"/>
+    <sheet name="advSearch_30_31_32" sheetId="39" r:id="rId38"/>
+    <sheet name="advSearch_039_040_041" sheetId="35" r:id="rId39"/>
+    <sheet name="advSearch_041" sheetId="36" r:id="rId40"/>
+    <sheet name="advSearch_042_043_044" sheetId="40" r:id="rId41"/>
+    <sheet name="deleteCreatedItem" sheetId="41" r:id="rId42"/>
+    <sheet name="deleteCreatedBrand" sheetId="42" r:id="rId43"/>
+    <sheet name="deleteCreatedSubset" sheetId="43" r:id="rId44"/>
+    <sheet name="advSearch_045_46" sheetId="37" r:id="rId45"/>
+    <sheet name="deleteCreatedManufactures" sheetId="44" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -63,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="185">
   <si>
     <t>User name</t>
   </si>
@@ -609,6 +618,15 @@
   </si>
   <si>
     <t>New Vendor saved Successfully</t>
+  </si>
+  <si>
+    <t>Vendor : '"+vendorName+"' removed Successfully</t>
+  </si>
+  <si>
+    <t>exp succes message</t>
+  </si>
+  <si>
+    <t>removeVendorTest</t>
   </si>
 </sst>
 </file>
@@ -691,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -722,6 +740,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1033,18 +1052,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1067,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1103,16 +1122,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1129,7 +1148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1159,17 +1178,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -1222,18 +1241,18 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1256,7 +1275,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1293,17 +1312,17 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -1356,16 +1375,16 @@
       <selection activeCell="A3" sqref="A3:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1382,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
@@ -1412,17 +1431,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1461,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -1475,17 +1494,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1524,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
@@ -1538,17 +1557,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -1601,17 +1620,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1650,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
@@ -1664,17 +1683,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1694,7 +1713,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1727,19 +1746,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1765,7 +1784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1804,16 +1823,16 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1855,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
@@ -1872,18 +1891,18 @@
       <selection activeCell="E1" sqref="E1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1906,7 +1925,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
@@ -1942,18 +1961,18 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1976,7 +1995,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -2012,17 +2031,17 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2064,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -2081,16 +2100,16 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2107,7 +2126,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -2124,7 +2143,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -2155,17 +2174,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2185,7 +2204,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -2218,16 +2237,16 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2244,7 +2263,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
@@ -2261,7 +2280,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>91</v>
       </c>
@@ -2278,7 +2297,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>92</v>
       </c>
@@ -2308,15 +2327,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2330,7 +2349,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -2357,15 +2376,15 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2379,7 +2398,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>92</v>
       </c>
@@ -2406,14 +2425,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2424,7 +2443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2448,17 +2467,17 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2478,7 +2497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2511,16 +2530,16 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2543,7 +2562,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -2566,7 +2585,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>95</v>
       </c>
@@ -2598,27 +2617,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G31" sqref="A3:XFD31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2675,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>165</v>
       </c>
@@ -2705,23 +2724,92 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="38.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="112.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2741,7 +2829,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2766,7 +2854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2774,18 +2862,18 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -2808,7 +2896,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>95</v>
       </c>
@@ -2831,7 +2919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>95</v>
       </c>
@@ -2854,7 +2942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>95</v>
       </c>
@@ -2883,7 +2971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2891,17 +2979,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2921,7 +3009,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2941,7 +3029,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
@@ -2966,7 +3054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2974,17 +3062,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3004,7 +3092,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>110</v>
       </c>
@@ -3024,7 +3112,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>132</v>
       </c>
@@ -3044,7 +3132,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>133</v>
       </c>
@@ -3069,7 +3157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3077,17 +3165,17 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3107,7 +3195,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
@@ -3127,7 +3215,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -3152,7 +3240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -3160,17 +3248,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="109.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3190,7 +3278,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -3208,7 +3296,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -3228,7 +3316,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>125</v>
       </c>
@@ -3251,7 +3339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -3259,18 +3347,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3293,7 +3381,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
@@ -3316,7 +3404,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
@@ -3339,7 +3427,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>113</v>
       </c>
@@ -3367,7 +3455,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -3375,17 +3565,17 @@
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3405,7 +3595,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>113</v>
       </c>
@@ -3425,7 +3615,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>113</v>
       </c>
@@ -3445,7 +3635,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>113</v>
       </c>
@@ -3465,7 +3655,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
@@ -3485,7 +3675,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>113</v>
       </c>
@@ -3510,28 +3700,260 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3545,33 +3967,12 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3582,55 +3983,36 @@
       <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="109.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3644,15 +4026,24 @@
         <v>96</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3664,15 +4055,24 @@
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -3684,57 +4084,115 @@
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="7" max="7" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+      <c r="E2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3745,21 +4203,15 @@
         <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3768,42 +4220,31 @@
         <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3813,19 +4254,62 @@
       <c r="C1" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3834,97 +4318,29 @@
         <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="109.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3935,27 +4351,15 @@
         <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
@@ -3964,147 +4368,35 @@
         <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="47" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -4115,217 +4407,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
code fixed for failures
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23160" windowHeight="12840" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23160" windowHeight="12840" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -4250,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4259,7 +4259,7 @@
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,7 +4287,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -4299,7 +4299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
items module fixed issues
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
+++ b/resources/ExcelsheetData/AdvancedSearchModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23160" windowHeight="12840" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23160" windowHeight="12840" firstSheet="35" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="createNewManufacturer" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="182">
   <si>
     <t>User name</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>TC_ADV SEARCH_006</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -2502,16 +2505,17 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3671,10 +3675,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3683,11 +3687,12 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3700,14 +3705,15 @@
       <c r="D1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>127</v>
       </c>
@@ -3721,13 +3727,16 @@
         <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>128</v>
       </c>
@@ -3741,13 +3750,16 @@
         <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>129</v>
       </c>
@@ -3761,10 +3773,13 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
+      <c r="G4" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4250,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>